<commit_message>
upd to initiate initiate vars from excel
</commit_message>
<xml_diff>
--- a/files_directories_naming.xlsx
+++ b/files_directories_naming.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\o.husiev@opendeusto.es\01_PHD_CODE\chapter_5\spain\to_github_bilbao_otxarkoaga\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oleksandr-MSI\Documentos\GitHub\spacer-hb-framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131AC655-E120-4C7A-8B3B-C49A25F5A187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{230288D8-39DA-4B1C-B18B-743A29DBC8D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A1B48F93-7407-4BBB-8927-FD6BF804E657}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>PATH</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>wb_rt_analysis_bilbao_otxarkoaga_segments.shp</t>
-  </si>
-  <si>
-    <t>D:\o.husiev@opendeusto.es\01_PHD_CODE\chapter_5\spain\</t>
   </si>
   <si>
     <t>otxarkoaga_pv.shp</t>
@@ -458,7 +455,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -469,19 +466,16 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -493,7 +487,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -501,15 +495,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -517,10 +511,10 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>